<commit_message>
starteTraining --> setStarten --> fortschrittEintragen
</commit_message>
<xml_diff>
--- a/FitnessApp-Daten.xlsx
+++ b/FitnessApp-Daten.xlsx
@@ -1,41 +1,73 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hatip\Documents\Visual Code\Python\FitnessApp\FitnessApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
   </bookViews>
   <sheets>
-    <sheet name="Uebungen" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Trainingsstatistiken" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Uebungen" sheetId="1" r:id="rId1"/>
+    <sheet name="Trainingsstatistiken" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+  <si>
+    <t>Uebung</t>
+  </si>
+  <si>
+    <t>Saetze</t>
+  </si>
+  <si>
+    <t>Wiederholungen</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Push Ups</t>
+  </si>
+  <si>
+    <t>Pull Ups</t>
+  </si>
+  <si>
+    <t>Squats</t>
+  </si>
+  <si>
+    <t>Deadlifts</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,17 +75,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -341,68 +392,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Uebung</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Saetze</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Wiederholungen</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>push ups</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>drei</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8 Uhr</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>pull UPS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -411,34 +466,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Datum</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>push ups</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>pull UPS</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>